<commit_message>
Updated file with Lat/Lon
File updated with Lat/Lon, Average home price and average income
</commit_message>
<xml_diff>
--- a/Voting .xlsx
+++ b/Voting .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/86f92d657950eb4f/Documents/BOOTCAMP/Multi-Axial Voter Participation Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA38793D-A5FB-452E-AF79-CC158528A8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A42C55D7-BDC3-4E41-9DC7-59FA5C25E62B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33390" yWindow="990" windowWidth="23010" windowHeight="12330" xr2:uid="{9BA252EA-C145-4054-BCD9-089B4472EA4C}"/>
+    <workbookView xWindow="29580" yWindow="1875" windowWidth="23010" windowHeight="12330" xr2:uid="{9BA252EA-C145-4054-BCD9-089B4472EA4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
   <si>
     <t># Voted</t>
   </si>
@@ -68,12 +68,18 @@
   <si>
     <t>133 ft</t>
   </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,16 +96,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
+      <sz val="11"/>
+      <color rgb="FF0066FF"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color rgb="FF0066FF"/>
-      <name val="Verdana"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -215,32 +216,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEEB4DE-183C-4AD4-AA36-31665BACE653}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,6 +571,9 @@
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" customWidth="1"/>
     <col min="5" max="7" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -588,11 +592,17 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="8" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -603,7 +613,7 @@
         <v>33535</v>
       </c>
       <c r="C2" s="5">
-        <f>SUM(D2:E2)</f>
+        <f t="shared" ref="C2:C21" si="0">SUM(D2:E2)</f>
         <v>33382</v>
       </c>
       <c r="D2" s="6">
@@ -612,22 +622,22 @@
       <c r="E2" s="6">
         <v>19267</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="7">
         <v>347700</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="7">
         <v>106560</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="8">
+      <c r="H2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="10">
         <v>28.067195999999999</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="10">
+      <c r="J2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="12">
         <v>-82.613676999999996</v>
       </c>
     </row>
@@ -639,7 +649,7 @@
         <v>24930</v>
       </c>
       <c r="C3" s="5">
-        <f>SUM(D3:E3)</f>
+        <f t="shared" si="0"/>
         <v>34542</v>
       </c>
       <c r="D3" s="6">
@@ -648,22 +658,22 @@
       <c r="E3" s="6">
         <v>19035</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="7">
         <v>492300</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="7">
         <v>115180</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="8">
+      <c r="H3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="10">
         <v>27.921807999999999</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="10">
+      <c r="J3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="12">
         <v>-82.508953000000005</v>
       </c>
     </row>
@@ -675,7 +685,7 @@
         <v>22560</v>
       </c>
       <c r="C4" s="5">
-        <f>SUM(D4:E4)</f>
+        <f t="shared" si="0"/>
         <v>19609</v>
       </c>
       <c r="D4" s="6">
@@ -684,10 +694,10 @@
       <c r="E4" s="6">
         <v>12141</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="7">
         <v>162400</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="7">
         <v>58013</v>
       </c>
       <c r="H4" s="13" t="s">
@@ -711,7 +721,7 @@
         <v>18517</v>
       </c>
       <c r="C5" s="5">
-        <f>SUM(D5:E5)</f>
+        <f t="shared" si="0"/>
         <v>18163</v>
       </c>
       <c r="D5" s="6">
@@ -720,22 +730,22 @@
       <c r="E5" s="6">
         <v>11050</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="7">
         <v>164700</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="7">
         <v>60267</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="8">
+      <c r="H5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="10">
         <v>28.016173999999999</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="10">
+      <c r="J5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="12">
         <v>-82.611958000000001</v>
       </c>
     </row>
@@ -747,7 +757,7 @@
         <v>18417</v>
       </c>
       <c r="C6" s="5">
-        <f>SUM(D6:E6)</f>
+        <f t="shared" si="0"/>
         <v>16651</v>
       </c>
       <c r="D6" s="6">
@@ -756,22 +766,22 @@
       <c r="E6" s="6">
         <v>10299</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="7">
         <v>146000</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="7">
         <v>52635</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="8">
+      <c r="H6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="10">
         <v>28.049979</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="J6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="12">
         <v>-82.363445999999996</v>
       </c>
     </row>
@@ -783,7 +793,7 @@
         <v>19376</v>
       </c>
       <c r="C7" s="5">
-        <f>SUM(D7:E7)</f>
+        <f t="shared" si="0"/>
         <v>25175</v>
       </c>
       <c r="D7" s="6">
@@ -792,22 +802,22 @@
       <c r="E7" s="6">
         <v>14845</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="7">
         <v>344500</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="7">
         <v>35770</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="8">
+      <c r="H7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="10">
         <v>27.770612</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="J7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="12">
         <v>-82.636238000000006</v>
       </c>
     </row>
@@ -815,9 +825,11 @@
       <c r="A8" s="4">
         <v>33801</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5">
+        <v>32970</v>
+      </c>
       <c r="C8" s="5">
-        <f>SUM(D8:E8)</f>
+        <f t="shared" si="0"/>
         <v>28474</v>
       </c>
       <c r="D8" s="6">
@@ -826,18 +838,22 @@
       <c r="E8" s="6">
         <v>17895</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="8">
+      <c r="F8" s="7">
+        <v>78700</v>
+      </c>
+      <c r="G8" s="7">
+        <v>35696</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="10">
         <v>28.042681000000002</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="10">
+      <c r="J8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="12">
         <v>-81.906626000000003</v>
       </c>
     </row>
@@ -845,9 +861,11 @@
       <c r="A9" s="4">
         <v>33803</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5">
+        <v>29675</v>
+      </c>
       <c r="C9" s="5">
-        <f>SUM(D9:E9)</f>
+        <f t="shared" si="0"/>
         <v>31091</v>
       </c>
       <c r="D9" s="6">
@@ -856,18 +874,22 @@
       <c r="E9" s="6">
         <v>17924</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="8">
+      <c r="F9" s="7">
+        <v>133100</v>
+      </c>
+      <c r="G9" s="7">
+        <v>51502</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="10">
         <v>28.015436999999999</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="10">
+      <c r="J9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="12">
         <v>-81.935204999999996</v>
       </c>
     </row>
@@ -875,9 +897,11 @@
       <c r="A10" s="4">
         <v>33805</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5">
+        <v>27347</v>
+      </c>
       <c r="C10" s="5">
-        <f>SUM(D10:E10)</f>
+        <f t="shared" si="0"/>
         <v>24203</v>
       </c>
       <c r="D10" s="6">
@@ -886,18 +910,22 @@
       <c r="E10" s="6">
         <v>15117</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="8">
+      <c r="F10" s="7">
+        <v>79900</v>
+      </c>
+      <c r="G10" s="7">
+        <v>35198</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="10">
         <v>-81.945372000000006</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -907,7 +935,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5">
-        <f>SUM(D11:E11)</f>
+        <f t="shared" si="0"/>
         <v>14475</v>
       </c>
       <c r="D11" s="6">
@@ -916,18 +944,18 @@
       <c r="E11" s="6">
         <v>649</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="8">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="10">
         <v>27.937799999999999</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="10">
+      <c r="J11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="12">
         <v>-82.286100000000005</v>
       </c>
     </row>
@@ -935,9 +963,11 @@
       <c r="A12" s="4">
         <v>33974</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5">
+        <v>17770</v>
+      </c>
       <c r="C12" s="5">
-        <f>SUM(D12:E12)</f>
+        <f t="shared" si="0"/>
         <v>11765</v>
       </c>
       <c r="D12" s="6">
@@ -946,18 +976,22 @@
       <c r="E12" s="6">
         <v>7558</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="8">
+      <c r="F12" s="7">
+        <v>145800</v>
+      </c>
+      <c r="G12" s="7">
+        <v>47831</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="10">
         <v>26.559547999999999</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" s="10">
+      <c r="J12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="12">
         <v>-81.613016000000002</v>
       </c>
     </row>
@@ -965,9 +999,11 @@
       <c r="A13" s="4">
         <v>33976</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5">
+        <v>17170</v>
+      </c>
       <c r="C13" s="5">
-        <f>SUM(D13:E13)</f>
+        <f t="shared" si="0"/>
         <v>10347</v>
       </c>
       <c r="D13" s="6">
@@ -976,18 +1012,22 @@
       <c r="E13" s="6">
         <v>6770</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="8">
+      <c r="F13" s="7">
+        <v>133300</v>
+      </c>
+      <c r="G13" s="7">
+        <v>48957</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="10">
         <v>26.586380999999999</v>
       </c>
-      <c r="J13" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" s="10">
+      <c r="J13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="12">
         <v>-81.687653999999995</v>
       </c>
     </row>
@@ -995,9 +1035,11 @@
       <c r="A14" s="4">
         <v>33980</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5">
+        <v>13407</v>
+      </c>
       <c r="C14" s="5">
-        <f>SUM(D14:E14)</f>
+        <f t="shared" si="0"/>
         <v>13897</v>
       </c>
       <c r="D14" s="6">
@@ -1006,8 +1048,12 @@
       <c r="E14" s="6">
         <v>7868</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="F14" s="7">
+        <v>140800</v>
+      </c>
+      <c r="G14" s="7">
+        <v>43559</v>
+      </c>
       <c r="H14" s="13" t="s">
         <v>5</v>
       </c>
@@ -1025,9 +1071,11 @@
       <c r="A15" s="4">
         <v>33981</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5">
+        <v>16212</v>
+      </c>
       <c r="C15" s="5">
-        <f>SUM(D15:E15)</f>
+        <f t="shared" si="0"/>
         <v>17565</v>
       </c>
       <c r="D15" s="6">
@@ -1036,18 +1084,22 @@
       <c r="E15" s="6">
         <v>9985</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" s="8">
+      <c r="F15" s="7">
+        <v>231300</v>
+      </c>
+      <c r="G15" s="7">
+        <v>54461</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="10">
         <v>26.930111</v>
       </c>
-      <c r="J15" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15" s="10">
+      <c r="J15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="12">
         <v>-82.215362999999996</v>
       </c>
     </row>
@@ -1055,9 +1107,11 @@
       <c r="A16" s="4">
         <v>33982</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5">
+        <v>12593</v>
+      </c>
       <c r="C16" s="5">
-        <f>SUM(D16:E16)</f>
+        <f t="shared" si="0"/>
         <v>12939</v>
       </c>
       <c r="D16" s="6">
@@ -1066,18 +1120,22 @@
       <c r="E16" s="6">
         <v>7470</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" s="8">
+      <c r="F16" s="7">
+        <v>113200</v>
+      </c>
+      <c r="G16" s="7">
+        <v>47067</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="10">
         <v>26.901980999999999</v>
       </c>
-      <c r="J16" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K16" s="10">
+      <c r="J16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="12">
         <v>-81.791608999999994</v>
       </c>
     </row>
@@ -1085,9 +1143,11 @@
       <c r="A17" s="4">
         <v>32664</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5">
+        <v>510</v>
+      </c>
       <c r="C17" s="5">
-        <f>SUM(D17:E17)</f>
+        <f t="shared" si="0"/>
         <v>788</v>
       </c>
       <c r="D17" s="6">
@@ -1096,28 +1156,34 @@
       <c r="E17" s="6">
         <v>448</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17" s="8">
+      <c r="F17" s="7">
+        <v>108100</v>
+      </c>
+      <c r="G17" s="7">
+        <v>44821</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="10">
         <v>29.441088000000001</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="10">
+      <c r="J17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="12">
         <v>-82.221224000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>32666</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5">
+        <v>5679</v>
+      </c>
       <c r="C18" s="5">
-        <f>SUM(D18:E18)</f>
+        <f t="shared" si="0"/>
         <v>7853</v>
       </c>
       <c r="D18" s="6">
@@ -1126,16 +1192,34 @@
       <c r="E18" s="6">
         <v>4479</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="7">
+        <v>136100</v>
+      </c>
+      <c r="G18" s="7">
+        <v>47067</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="10">
+        <v>29.724643</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="12">
+        <v>-82.002427999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>32667</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5">
+        <v>3649</v>
+      </c>
       <c r="C19" s="5">
-        <f>SUM(D19:E19)</f>
+        <f t="shared" si="0"/>
         <v>5447</v>
       </c>
       <c r="D19" s="6">
@@ -1144,16 +1228,34 @@
       <c r="E19" s="6">
         <v>3046</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="7">
+        <v>236200</v>
+      </c>
+      <c r="G19" s="7">
+        <v>52500</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="10">
+        <v>29.552447000000001</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="12">
+        <v>-82.313962000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>32668</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="5">
+        <v>6019</v>
+      </c>
       <c r="C20" s="5">
-        <f>SUM(D20:E20)</f>
+        <f t="shared" si="0"/>
         <v>6317</v>
       </c>
       <c r="D20" s="6">
@@ -1162,16 +1264,34 @@
       <c r="E20" s="6">
         <v>3656</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="7">
+        <v>153500</v>
+      </c>
+      <c r="G20" s="7">
+        <v>39277</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="10">
+        <v>29.254058000000001</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="12">
+        <v>-82.52816</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>32669</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5">
+        <v>15554</v>
+      </c>
       <c r="C21" s="5">
-        <f>SUM(D21:E21)</f>
+        <f t="shared" si="0"/>
         <v>18531</v>
       </c>
       <c r="D21" s="6">
@@ -1180,8 +1300,24 @@
       <c r="E21" s="6">
         <v>10518</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="F21" s="7">
+        <v>197900</v>
+      </c>
+      <c r="G21" s="7">
+        <v>69439</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="10">
+        <v>29.631326999999999</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="12">
+        <v>-82.581421000000006</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>